<commit_message>
Refactor ExcelReader.js and remove unused excelReader.js file
</commit_message>
<xml_diff>
--- a/src/utils/spreadsheets/week 11.xlsx
+++ b/src/utils/spreadsheets/week 11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordy\pick-em-1\src\utils\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51F05FFF-1B93-49D6-B52C-88753361E803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F264EA-5803-4BB2-8A9B-ACEBC1470949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{506D9C36-05BF-40C5-908D-2C62F6C0E612}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="56">
   <si>
     <t>Away</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>DONTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buccaneers </t>
   </si>
 </sst>
 </file>
@@ -667,7 +670,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,6 +682,7 @@
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -922,7 +926,7 @@
         <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="L5" t="s">
         <v>26</v>

</xml_diff>